<commit_message>
Ahora funciona para tarde y noche
</commit_message>
<xml_diff>
--- a/Tablas-copia.xlsx
+++ b/Tablas-copia.xlsx
@@ -14,39 +14,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Aulas</t>
   </si>
   <si>
-    <t>07:30:00</t>
-  </si>
-  <si>
-    <t>08:00:00</t>
-  </si>
-  <si>
-    <t>08:30:00</t>
-  </si>
-  <si>
-    <t>09:00:00</t>
-  </si>
-  <si>
-    <t>09:30:00</t>
-  </si>
-  <si>
-    <t>10:00:00</t>
-  </si>
-  <si>
-    <t>10:30:00</t>
-  </si>
-  <si>
-    <t>11:00:00</t>
-  </si>
-  <si>
-    <t>11:30:00</t>
-  </si>
-  <si>
-    <t>12:00:00</t>
+    <t>12:30:00</t>
+  </si>
+  <si>
+    <t>13:00:00</t>
+  </si>
+  <si>
+    <t>13:30:00</t>
+  </si>
+  <si>
+    <t>14:00:00</t>
+  </si>
+  <si>
+    <t>14:30:00</t>
+  </si>
+  <si>
+    <t>15:00:00</t>
+  </si>
+  <si>
+    <t>15:30:00</t>
+  </si>
+  <si>
+    <t>16:00:00</t>
+  </si>
+  <si>
+    <t>16:30:00</t>
+  </si>
+  <si>
+    <t>17:00:00</t>
+  </si>
+  <si>
+    <t>17:30:00</t>
   </si>
   <si>
     <t>AUDITORIO COMPLETO</t>
@@ -533,13 +536,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -573,10 +576,13 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -591,62 +597,68 @@
         <v>1</v>
       </c>
       <c r="F2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>0</v>
+      </c>
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -667,21 +679,24 @@
         <v>1</v>
       </c>
       <c r="H4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>0</v>
+      </c>
+      <c r="L4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -713,10 +728,13 @@
       <c r="K5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -748,10 +766,13 @@
       <c r="K6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -772,21 +793,24 @@
         <v>1</v>
       </c>
       <c r="H7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -807,21 +831,24 @@
         <v>1</v>
       </c>
       <c r="H8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -853,10 +880,13 @@
       <c r="K9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -877,21 +907,24 @@
         <v>1</v>
       </c>
       <c r="H10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -923,10 +956,13 @@
       <c r="K11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
@@ -947,39 +983,42 @@
         <v>1</v>
       </c>
       <c r="H12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -993,10 +1032,13 @@
       <c r="K13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="L13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -1017,21 +1059,24 @@
         <v>1</v>
       </c>
       <c r="H14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>0</v>
+      </c>
+      <c r="L14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -1052,39 +1097,42 @@
         <v>1</v>
       </c>
       <c r="H15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>0</v>
+      </c>
+      <c r="L15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
@@ -1098,10 +1146,13 @@
       <c r="K16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -1133,10 +1184,13 @@
       <c r="K17" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
@@ -1168,10 +1222,13 @@
       <c r="K18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -1186,10 +1243,10 @@
         <v>1</v>
       </c>
       <c r="F19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
@@ -1203,10 +1260,13 @@
       <c r="K19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
@@ -1227,21 +1287,24 @@
         <v>1</v>
       </c>
       <c r="H20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+        <v>0</v>
+      </c>
+      <c r="L20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -1273,10 +1336,13 @@
       <c r="K21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="L21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" t="b">
         <v>1</v>
@@ -1308,10 +1374,13 @@
       <c r="K22" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="L22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B23" t="b">
         <v>1</v>
@@ -1326,27 +1395,30 @@
         <v>1</v>
       </c>
       <c r="F23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
@@ -1361,27 +1433,30 @@
         <v>1</v>
       </c>
       <c r="F24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+        <v>0</v>
+      </c>
+      <c r="L24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
@@ -1413,10 +1488,13 @@
       <c r="K25" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="L25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B26" t="b">
         <v>1</v>
@@ -1431,27 +1509,30 @@
         <v>1</v>
       </c>
       <c r="F26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B27" t="b">
         <v>1</v>
@@ -1466,10 +1547,10 @@
         <v>1</v>
       </c>
       <c r="F27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" t="b">
         <v>0</v>
@@ -1483,10 +1564,13 @@
       <c r="K27" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="L27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B28" t="b">
         <v>1</v>
@@ -1507,21 +1591,24 @@
         <v>1</v>
       </c>
       <c r="H28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+        <v>0</v>
+      </c>
+      <c r="L28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
@@ -1536,27 +1623,30 @@
         <v>1</v>
       </c>
       <c r="F29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B30" t="b">
         <v>1</v>
@@ -1588,10 +1678,13 @@
       <c r="K30" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="L30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
@@ -1612,21 +1705,24 @@
         <v>1</v>
       </c>
       <c r="H31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
@@ -1647,21 +1743,24 @@
         <v>1</v>
       </c>
       <c r="H32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+        <v>0</v>
+      </c>
+      <c r="L32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B33" t="b">
         <v>1</v>
@@ -1676,27 +1775,30 @@
         <v>1</v>
       </c>
       <c r="F33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K33" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+        <v>0</v>
+      </c>
+      <c r="L33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B34" t="b">
         <v>1</v>
@@ -1728,10 +1830,13 @@
       <c r="K34" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:11">
+      <c r="L34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B35" t="b">
         <v>1</v>
@@ -1752,21 +1857,24 @@
         <v>1</v>
       </c>
       <c r="H35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
+        <v>0</v>
+      </c>
+      <c r="L35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B36" t="b">
         <v>1</v>
@@ -1781,27 +1889,30 @@
         <v>1</v>
       </c>
       <c r="F36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K36" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
+        <v>0</v>
+      </c>
+      <c r="L36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B37" t="b">
         <v>1</v>
@@ -1833,10 +1944,13 @@
       <c r="K37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="L37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B38" t="b">
         <v>1</v>
@@ -1868,10 +1982,13 @@
       <c r="K38" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:11">
+      <c r="L38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B39" t="b">
         <v>1</v>
@@ -1903,10 +2020,13 @@
       <c r="K39" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:11">
+      <c r="L39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B40" t="b">
         <v>1</v>
@@ -1938,10 +2058,13 @@
       <c r="K40" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:11">
+      <c r="L40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B41" t="b">
         <v>1</v>
@@ -1956,10 +2079,10 @@
         <v>1</v>
       </c>
       <c r="F41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41" t="b">
         <v>0</v>
@@ -1973,10 +2096,13 @@
       <c r="K41" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:11">
+      <c r="L41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B42" t="b">
         <v>1</v>
@@ -2008,10 +2134,13 @@
       <c r="K42" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="L42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B43" t="b">
         <v>1</v>
@@ -2032,21 +2161,24 @@
         <v>1</v>
       </c>
       <c r="H43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="L43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B44" t="b">
         <v>1</v>
@@ -2077,6 +2209,9 @@
       </c>
       <c r="K44" t="b">
         <v>1</v>
+      </c>
+      <c r="L44" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>